<commit_message>
cleaned up data frame.  need to work on angular
</commit_message>
<xml_diff>
--- a/src/python/rekogfiles.xlsx
+++ b/src/python/rekogfiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,16 @@
           <t>src</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>labels</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -446,7 +456,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[911f7cc1-3b0a-4807-8f0b-27a439ab12ferekogimages/.jpg,meeting.jpg,['Adult', 'Male', 'Man', 'Person', 'Conversation']]</t>
+          <t>911f7cc1-3b0a-4807-8f0b-27a439ab12fe.jpg</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>meeting.jpg</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['Adult', 'Male', 'Man', 'Person', 'Conversation']</t>
         </is>
       </c>
     </row>
@@ -456,7 +476,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[952e0e61-2748-48e2-a27c-57ec3a9c00e9rekogimages/.jpg,fatherson.jpg,['People', 'Person', 'Head', 'Face', 'Clothing', 'Footwear', 'Shoe']]</t>
+          <t>952e0e61-2748-48e2-a27c-57ec3a9c00e9.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>fatherson.jpg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['People', 'Person', 'Head', 'Face', 'Clothing', 'Footwear', 'Shoe']</t>
         </is>
       </c>
     </row>
@@ -466,7 +496,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[bd7b45c0-5e60-4916-b4c1-fa93df39bbb6rekogimages/.jpg,51874794015_50bd3f9f82_k.jpeg,['Adult', 'Male', 'Man', 'Person', 'Clothing', 'Footwear', 'Shoe', 'Wristwatch', 'Police', 'People', 'Accessories', 'Glasses', 'Officer', 'Police Officer', 'Bag', 'Handbag', 'Gun', 'Weapon']]</t>
+          <t>bd7b45c0-5e60-4916-b4c1-fa93df39bbb6.jpg</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>51874794015_50bd3f9f82_k.jpeg</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['Adult', 'Male', 'Man', 'Person', 'Clothing', 'Footwear', 'Shoe', 'Wristwatch', 'Police', 'People', 'Accessories', 'Glasses', 'Officer', 'Police Officer', 'Bag', 'Handbag', 'Gun', 'Weapon']</t>
         </is>
       </c>
     </row>

</xml_diff>